<commit_message>
varun kumar a paid the fees
</commit_message>
<xml_diff>
--- a/sampleworksheet.xlsx
+++ b/sampleworksheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>S.No</t>
   </si>
@@ -25,12 +25,6 @@
   </si>
   <si>
     <t>Name</t>
-  </si>
-  <si>
-    <t>18bec048</t>
-  </si>
-  <si>
-    <t>VARUN KUMAR A</t>
   </si>
   <si>
     <t>19bcs001</t>
@@ -478,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -502,7 +496,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -513,7 +507,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
@@ -524,7 +518,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -535,7 +529,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -546,7 +540,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
@@ -556,8 +550,8 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="4">
-        <v>6</v>
+      <c r="A7" s="6">
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
@@ -567,8 +561,8 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="6">
-        <v>7</v>
+      <c r="A8" s="4">
+        <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>15</v>
@@ -579,7 +573,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>17</v>
@@ -590,7 +584,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>19</v>
@@ -601,7 +595,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>21</v>
@@ -612,7 +606,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>23</v>
@@ -623,30 +617,19 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="4">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>$B$2:$B$1209</formula1>
+      <formula1>$B$2:$B$1208</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>